<commit_message>
edit export data excel
</commit_message>
<xml_diff>
--- a/export-excel/templates/audit.xlsx
+++ b/export-excel/templates/audit.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\SINERGI\export-excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDB027C-CD3A-4020-92ED-154E013C7BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490E38E9-4E83-4498-B38F-9055F514E3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defect Keseluruhan" sheetId="1" r:id="rId1"/>
-    <sheet name="example" sheetId="2" r:id="rId2"/>
+    <sheet name="template" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Defect Keseluruhan'!$A$8:$F$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">example!$A$9:$G$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">template!$A$9:$G$40</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>FORM GENERAL CHECK LIFT PT. SINERGI KARYA MANDIRI</t>
   </si>
@@ -75,10 +75,16 @@
     <t>MESIN ROOM</t>
   </si>
   <si>
-    <t>: LS</t>
-  </si>
-  <si>
-    <t>: 30 Mei2024</t>
+    <t xml:space="preserve"> : Metropolitan Mall Cikarang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> : P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> : Jl. Surakarta. No.2 Surabaya </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> : 2024-12-18 21:09:49</t>
   </si>
   <si>
     <t>Number Picture</t>
@@ -91,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,8 +121,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,8 +154,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFEEEE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -185,11 +216,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -209,12 +282,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -225,12 +292,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{595E1CB9-6E0F-4972-AF50-DA64A8458C34}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -505,11 +600,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="9" topLeftCell="D37" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11:A59"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -524,15 +619,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="3" spans="1:9">
       <c r="B3" t="s">
@@ -544,10 +639,10 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="12"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:9">
       <c r="B4" t="s">
@@ -559,38 +654,38 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
@@ -1054,262 +1149,263 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDAE332-FEB7-4019-964C-29642A2634C2}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="9" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="43.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="9" style="14"/>
+    <col min="4" max="4" width="31.140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="43.85546875" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="12"/>
+      <c r="F3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" t="s">
+      <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="12"/>
+      <c r="F4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="16"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>19</v>
+      <c r="F8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="5"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="9"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="A11" s="23"/>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="A12" s="23"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="A13" s="23"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="A14" s="23"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="A15" s="23"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="A16" s="23"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" s="1" customFormat="1">
-      <c r="A18" s="7"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" s="1" customFormat="1">
-      <c r="A19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1">
-      <c r="A20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" s="1" customFormat="1">
-      <c r="A21" s="7"/>
-      <c r="G21" s="7"/>
+      <c r="A17" s="23"/>
+      <c r="G17" s="23"/>
+    </row>
+    <row r="18" spans="1:7" s="24" customFormat="1">
+      <c r="A18" s="23"/>
+      <c r="G18" s="23"/>
+    </row>
+    <row r="19" spans="1:7" s="24" customFormat="1">
+      <c r="A19" s="23"/>
+      <c r="G19" s="23"/>
+    </row>
+    <row r="20" spans="1:7" s="24" customFormat="1">
+      <c r="A20" s="23"/>
+      <c r="G20" s="23"/>
+    </row>
+    <row r="21" spans="1:7" s="24" customFormat="1">
+      <c r="A21" s="23"/>
+      <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="7"/>
-      <c r="G22" s="7"/>
+      <c r="A22" s="23"/>
+      <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="7"/>
-      <c r="G23" s="7"/>
+      <c r="A23" s="23"/>
+      <c r="G23" s="23"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="7"/>
-      <c r="G24" s="7"/>
+      <c r="A24" s="23"/>
+      <c r="G24" s="23"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="A25" s="23"/>
+      <c r="G25" s="23"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="7"/>
-      <c r="G26" s="7"/>
+      <c r="A26" s="23"/>
+      <c r="G26" s="23"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="7"/>
-      <c r="G27" s="7"/>
+      <c r="A27" s="23"/>
+      <c r="G27" s="23"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="7"/>
-      <c r="G28" s="7"/>
+      <c r="A28" s="23"/>
+      <c r="G28" s="23"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="7"/>
-      <c r="G29" s="7"/>
+      <c r="A29" s="23"/>
+      <c r="G29" s="23"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="7"/>
-      <c r="G30" s="7"/>
+      <c r="A30" s="23"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="7"/>
-      <c r="G31" s="7"/>
+      <c r="A31" s="23"/>
+      <c r="G31" s="23"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="7"/>
-      <c r="G32" s="7"/>
+      <c r="A32" s="23"/>
+      <c r="G32" s="23"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="7"/>
-      <c r="G33" s="7"/>
+      <c r="A33" s="23"/>
+      <c r="G33" s="23"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="7"/>
-      <c r="G34" s="7"/>
+      <c r="A34" s="23"/>
+      <c r="G34" s="23"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="7"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" s="1" customFormat="1">
-      <c r="A36" s="7"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" s="1" customFormat="1">
-      <c r="A37" s="7"/>
-      <c r="G37" s="7"/>
+      <c r="A35" s="23"/>
+      <c r="G35" s="23"/>
+    </row>
+    <row r="36" spans="1:7" s="24" customFormat="1">
+      <c r="A36" s="23"/>
+      <c r="G36" s="23"/>
+    </row>
+    <row r="37" spans="1:7" s="24" customFormat="1">
+      <c r="A37" s="23"/>
+      <c r="G37" s="23"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="7"/>
-      <c r="G38" s="7"/>
+      <c r="A38" s="23"/>
+      <c r="G38" s="23"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="7"/>
-      <c r="G39" s="7"/>
-    </row>
-    <row r="40" spans="1:7" s="1" customFormat="1">
-      <c r="A40" s="7"/>
-      <c r="G40" s="7"/>
+      <c r="A39" s="23"/>
+      <c r="G39" s="23"/>
+    </row>
+    <row r="40" spans="1:7" s="24" customFormat="1">
+      <c r="A40" s="23"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="7"/>
-      <c r="G41" s="7"/>
+      <c r="A41" s="23"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="7"/>
-      <c r="G42" s="7"/>
+      <c r="A42" s="23"/>
+      <c r="G42" s="23"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="7"/>
+      <c r="A43" s="23"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="7"/>
+      <c r="A44" s="23"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="7"/>
+      <c r="A45" s="23"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="7"/>
+      <c r="A46" s="23"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="7"/>
+      <c r="A47" s="23"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="7"/>
+      <c r="A48" s="23"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="7"/>
+      <c r="A49" s="23"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="7"/>
+      <c r="A50" s="23"/>
     </row>
   </sheetData>
   <autoFilter ref="A9:G40" xr:uid="{00000000-0009-0000-0000-000001000000}"/>

</xml_diff>